<commit_message>
Corregir el error del reset, ahora al hacer reset se vuelve a llamar a fetch para cargar las tasas
</commit_message>
<xml_diff>
--- a/assets/model/Calculadora de divisas.xlsx
+++ b/assets/model/Calculadora de divisas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iteca-Programador\Downloads\Manuel_Henriquez\Pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iteca-Programador\Downloads\Manuel_Henriquez\Pruebas\mh-calculadora-divisas\assets\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B0CFB7-106B-4730-9C7F-4CEA9453980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B2C05B-9DA9-42FB-82C7-538334F4C95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2190" yWindow="450" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculadora en $" sheetId="9" r:id="rId1"/>
@@ -392,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D7EB60-92FE-4710-8DBA-06E2CE4339D0}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -578,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Selector para tomar la base en dolares y bolivares funcionalidad terminada
</commit_message>
<xml_diff>
--- a/assets/model/Calculadora de divisas.xlsx
+++ b/assets/model/Calculadora de divisas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iteca-Programador\Downloads\Manuel_Henriquez\Pruebas\mh-calculadora-divisas\assets\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B2C05B-9DA9-42FB-82C7-538334F4C95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2740DB81-EAD8-4A99-B744-3E7824E3A6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="450" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="1365" windowWidth="15375" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculadora en $" sheetId="9" r:id="rId1"/>
@@ -393,7 +393,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -579,7 +579,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Redondeo con precisión 2 decimales terminado, se hicieron pruebas con excel y los cálculos son exactos como los daba anterior a estos cambios, se recomienda validar si integrar esta rama
</commit_message>
<xml_diff>
--- a/assets/model/Calculadora de divisas.xlsx
+++ b/assets/model/Calculadora de divisas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iteca-Programador\Downloads\Manuel_Henriquez\Pruebas\mh-calculadora-divisas\assets\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2740DB81-EAD8-4A99-B744-3E7824E3A6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F4818A-D6B0-408A-9674-536AF8484C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="1365" windowWidth="15375" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4230" yWindow="1380" windowWidth="14820" windowHeight="7260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculadora en $" sheetId="9" r:id="rId1"/>
@@ -392,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D7EB60-92FE-4710-8DBA-06E2CE4339D0}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -578,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>

</xml_diff>